<commit_message>
Added Get annotations to desearialize models
</commit_message>
<xml_diff>
--- a/FilesOrganizerIDOffice/src/main/resources/una/filesorganizeridoffice/xlsx/Formato Individual Menores.xlsx
+++ b/FilesOrganizerIDOffice/src/main/resources/una/filesorganizeridoffice/xlsx/Formato Individual Menores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\FileOrganizer\FilesOrganizerIDOffice\src\main\resources\una\filesorganizeridoffice\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\N00148095\Desktop\Git\FileOrganizer\FilesOrganizerIDOffice\src\main\resources\una\filesorganizeridoffice\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51859D6-1657-4BC6-95A4-66D2EF974F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBCA854-9DD8-47D3-9820-2DE9225D4FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="0" windowWidth="10620" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Tipo ID</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Fecha nacimiento</t>
-  </si>
-  <si>
-    <t>Oficina (punto de entrega)</t>
   </si>
   <si>
     <t>Tipo ID del autorizado</t>
@@ -454,13 +451,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
@@ -471,30 +468,29 @@
     <col min="7" max="7" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="30.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="29.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="30.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
@@ -509,19 +505,19 @@
         <v>4</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>6</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>19</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>7</v>
@@ -536,19 +532,19 @@
         <v>10</v>
       </c>
       <c r="P1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>12</v>
       </c>
       <c r="S1" s="8" t="s">
         <v>21</v>
       </c>
       <c r="T1" s="8" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="U1" s="8" t="s">
         <v>13</v>
@@ -562,11 +558,8 @@
       <c r="X1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="Y1" s="8" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -576,22 +569,21 @@
       <c r="G2" s="7"/>
       <c r="H2" s="2"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="5"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="7"/>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="7"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="5"/>
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="5"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>